<commit_message>
add header and background
</commit_message>
<xml_diff>
--- a/Client/data/content.xlsx
+++ b/Client/data/content.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Javascript\Website\Quan\Client\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA40B64-F162-4528-9992-501C6A392A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDA587C-2EF9-426D-BE6E-305DCC2C4557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="540" yWindow="1152" windowWidth="11508" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,9 +55,6 @@
     <t>Header_3</t>
   </si>
   <si>
-    <t>Our Service</t>
-  </si>
-  <si>
     <t>Liên Hệ</t>
   </si>
   <si>
@@ -92,6 +89,9 @@
   </si>
   <si>
     <t>EN</t>
+  </si>
+  <si>
+    <t>Our Services</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,13 +446,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -460,10 +460,10 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -471,10 +471,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -482,18 +482,18 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -501,10 +501,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>

</xml_diff>